<commit_message>
feat: add cach_flow data , dividend data
</commit_message>
<xml_diff>
--- a/2330_台積電_財務分析報告_20250725.xlsx
+++ b/2330_台積電_財務分析報告_20250725.xlsx
@@ -12,7 +12,11 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="季度財務" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="年度財務" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="股利政策" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="潛力分析" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="現金流量" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="除權除息結果" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="股價分析" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="財務比率" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="潛力分析" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -644,6 +648,138 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>潛力股分析</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>總分</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>92.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>評等</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>A+</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>成長潛力</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>100.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>獲利能力</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>穩定性</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>估值合理性</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>配息穩定性</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>分析日期</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -1906,7 +2042,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1927,101 +2063,487 @@
     <row r="1">
       <c r="A1" s="4" t="inlineStr">
         <is>
-          <t>潛力股分析</t>
+          <t>近8季現金流量資料</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>無現金流量資料</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>近5年除權除息結果</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>無除權除息結果資料</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>股價技術分析</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>總分</t>
+          <t>當前股價</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>92.0</t>
+          <t>1145.00</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>評等</t>
+          <t>52週最高</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>A+</t>
+          <t>1160.00</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>成長潛力</t>
+          <t>52週最低</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>100.0</t>
+          <t>780.00</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>獲利能力</t>
+          <t>平均成交量</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>無資料</t>
+          <t>41,087,723</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>穩定性</t>
+          <t>股價波動率</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>無資料</t>
+          <t>7.63%</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>估值合理性</t>
+          <t>近期趨勢</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
+          <t>上升</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>財務比率分析</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>日期</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>流動比率</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>速動比率</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>負債比率</t>
+        </is>
+      </c>
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t>營業現金流</t>
+        </is>
+      </c>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>現金流量品質</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="D4" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="E4" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="F4" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>2024-12-31</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="D5" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="F5" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="C6" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="D6" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="E6" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="F6" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>2024-06-30</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="C7" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="D7" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="E7" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="F7" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>2024-03-31</t>
+        </is>
+      </c>
+      <c r="B8" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="C8" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="D8" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="E8" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="F8" s="6" t="inlineStr">
+        <is>
           <t>無資料</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="inlineStr">
-        <is>
-          <t>配息穩定性</t>
-        </is>
-      </c>
-      <c r="B9" s="3" t="inlineStr">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>2023-12-31</t>
+        </is>
+      </c>
+      <c r="B9" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="C9" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="D9" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="E9" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="F9" s="6" t="inlineStr">
         <is>
           <t>無資料</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>分析日期</t>
-        </is>
-      </c>
-      <c r="B10" s="3" t="inlineStr">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>2023-09-30</t>
+        </is>
+      </c>
+      <c r="B10" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="C10" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="D10" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="E10" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="F10" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>2023-06-30</t>
+        </is>
+      </c>
+      <c r="B11" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="C11" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="D11" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="E11" s="6" t="inlineStr">
+        <is>
+          <t>無資料</t>
+        </is>
+      </c>
+      <c r="F11" s="6" t="inlineStr">
         <is>
           <t>無資料</t>
         </is>

</xml_diff>